<commit_message>
day 28 write dat into excel
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufjon/IdeaProjects/va-spring-2019-selenium-testng/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vfomiuk/IdeaProjects/Fall2019Selenium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDDC9C1-934F-044B-80DB-58DA20C1AFF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25943BE8-09D8-114D-B59C-FE772C3C5EDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41120" yWindow="1540" windowWidth="33600" windowHeight="18920" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
+    <workbookView xWindow="3400" yWindow="29260" windowWidth="28800" windowHeight="16740" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="QA1-all" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3926" uniqueCount="1480">
   <si>
     <t>username</t>
   </si>
@@ -4470,12 +4470,19 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4829,8 +4836,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9073,8 +9080,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -9412,8 +9419,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -13659,8 +13666,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -13998,8 +14005,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -18240,13 +18247,14 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -18286,7 +18294,7 @@
         <v>305</v>
       </c>
       <c r="F2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -18306,7 +18314,7 @@
         <v>725</v>
       </c>
       <c r="F3" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -18326,7 +18334,7 @@
         <v>307</v>
       </c>
       <c r="F4" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -18346,7 +18354,7 @@
         <v>610</v>
       </c>
       <c r="F5" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -18366,7 +18374,7 @@
         <v>1021</v>
       </c>
       <c r="F6" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -18386,7 +18394,7 @@
         <v>1274</v>
       </c>
       <c r="F7" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -18406,7 +18414,7 @@
         <v>337</v>
       </c>
       <c r="F8" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -18426,7 +18434,7 @@
         <v>796</v>
       </c>
       <c r="F9" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -18446,7 +18454,7 @@
         <v>644</v>
       </c>
       <c r="F10" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -18466,7 +18474,7 @@
         <v>586</v>
       </c>
       <c r="F11" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -18486,7 +18494,7 @@
         <v>1375</v>
       </c>
       <c r="F12" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -18506,7 +18514,7 @@
         <v>1001</v>
       </c>
       <c r="F13" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -18526,7 +18534,7 @@
         <v>1378</v>
       </c>
       <c r="F14" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -18546,7 +18554,7 @@
         <v>1379</v>
       </c>
       <c r="F15" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -18566,7 +18574,7 @@
         <v>1381</v>
       </c>
       <c r="F16" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>